<commit_message>
Added Months to COD in the Technical Proposal document and updated PCS Voltage
</commit_message>
<xml_diff>
--- a/src/PCS.xlsx
+++ b/src/PCS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/DeployWithRender/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{473B8273-ECA8-47BB-891B-8B623FF00EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B06332C-3350-4B6B-9AE7-24B3C7A685E4}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{473B8273-ECA8-47BB-891B-8B623FF00EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3025A349-EA77-444D-AC9D-CA295603AEC4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E20" sqref="E20"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
         <v>800</v>
       </c>
       <c r="C10">
-        <v>800</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
PCS changes with duration
</commit_message>
<xml_diff>
--- a/src/PCS.xlsx
+++ b/src/PCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prevalonenergy-my.sharepoint.com/personal/himanshu_prevalonenergy_com/Documents/I drive/Sizing Tool/DeployWithRender/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{473B8273-ECA8-47BB-891B-8B623FF00EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3025A349-EA77-444D-AC9D-CA295603AEC4}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{473B8273-ECA8-47BB-891B-8B623FF00EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C02195BD-19C2-46D0-B039-FAE932814E80}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Model</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Sungrow SC5000UD-MV-US</t>
+  </si>
+  <si>
+    <t>Sungrow SC2750UD-MV-US</t>
   </si>
 </sst>
 </file>
@@ -118,9 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,89 +406,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C11" sqref="C11"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
+        <v>2750</v>
+      </c>
+      <c r="C2">
         <v>4000</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
+        <v>2750</v>
+      </c>
+      <c r="C3">
         <v>4000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
+        <v>2750</v>
+      </c>
+      <c r="C4">
         <v>4000</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>5000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <f>0.909*B4</f>
+        <v>2499.75</v>
+      </c>
+      <c r="C5">
+        <f>0.909*C4</f>
         <v>3636</v>
       </c>
-      <c r="C5">
-        <f>0.9*C4</f>
+      <c r="D5">
+        <f>0.9*D4</f>
         <v>4500</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
+        <v>800</v>
+      </c>
+      <c r="C6">
         <v>1150</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -494,8 +515,11 @@
       <c r="C7">
         <v>1500</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -505,8 +529,11 @@
       <c r="C8">
         <v>250000</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -516,30 +543,46 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
+        <v>550</v>
+      </c>
+      <c r="C10">
         <v>800</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>690</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
+        <f>C11</f>
         <v>0.98399999999999999</v>
       </c>
       <c r="C11" s="1">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="D11" s="1">
         <v>0.98399999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{defa4170-0d19-0005-0004-bc88714345d2}" enabled="1" method="Standard" siteId="{fda0a4a7-3813-444d-808d-54bb327d0367}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>